<commit_message>
Insert Logging to project
</commit_message>
<xml_diff>
--- a/src/main/resources/universityStatistics.xlsx
+++ b/src/main/resources/universityStatistics.xlsx
@@ -29,10 +29,10 @@
     <t>Universities names</t>
   </si>
   <si>
-    <t>LINGUISTICS</t>
+    <t>MEDICINE</t>
   </si>
   <si>
-    <t>ВЛПУ</t>
+    <t>МГМУ;ТУМ;СМИ</t>
   </si>
   <si>
     <t>PHYSICS</t>
@@ -41,16 +41,16 @@
     <t>МВУ;МПИ</t>
   </si>
   <si>
+    <t>LINGUISTICS</t>
+  </si>
+  <si>
+    <t>ВЛПУ</t>
+  </si>
+  <si>
     <t>MATHEMATICS</t>
   </si>
   <si>
     <t>КУВ</t>
-  </si>
-  <si>
-    <t>MEDICINE</t>
-  </si>
-  <si>
-    <t>МГМУ;ТУМ;СМИ</t>
   </si>
 </sst>
 </file>
@@ -129,13 +129,13 @@
         <v>5</v>
       </c>
       <c r="B2" t="n">
-        <v>0.0</v>
+        <v>4.329999923706055</v>
       </c>
       <c r="C2" t="n">
-        <v>1.0</v>
+        <v>3.0</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0</v>
+        <v>3.0</v>
       </c>
       <c r="E2" t="s">
         <v>6</v>
@@ -180,13 +180,13 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>4.329999923706055</v>
+        <v>0.0</v>
       </c>
       <c r="C5" t="n">
-        <v>3.0</v>
+        <v>1.0</v>
       </c>
       <c r="D5" t="n">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="E5" t="s">
         <v>12</v>

</xml_diff>